<commit_message>
extended report additional settings added
</commit_message>
<xml_diff>
--- a/Stat reports/Reports/Templates/Численность 6-Т для ПЭО.xlsx
+++ b/Stat reports/Reports/Templates/Численность 6-Т для ПЭО.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Stat reports\Stat reports\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3040FEA5-6910-4731-BCC9-42FB8E3C832D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832D940-3040-4D44-B243-98D452F431C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="19440" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,6 +327,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,18 +342,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -690,7 +694,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C47"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,20 +713,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -734,15 +738,15 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -752,19 +756,19 @@
         <f t="shared" ref="B3:B45" si="0">D3+E3+F3+G3+H3+I3+J3+L3+K3</f>
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="e">
+      <c r="C3" s="12" t="e">
         <f>SUM(B3:B14)/B48</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -774,16 +778,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -793,16 +797,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -812,16 +816,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -831,16 +835,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -850,16 +854,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -869,16 +873,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -888,16 +892,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -907,16 +911,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -926,16 +930,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -945,16 +949,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -964,16 +968,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -983,19 +987,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C15" s="9" t="e">
+      <c r="C15" s="11" t="e">
         <f>SUM(B15:B21)/B48</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1005,16 +1009,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1024,16 +1028,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1043,16 +1047,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1062,16 +1066,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1081,16 +1085,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
     </row>
     <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1100,16 +1104,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
     </row>
     <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1119,19 +1123,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C22" s="9" t="e">
+      <c r="C22" s="11" t="e">
         <f>SUM(B22:B47)/B48</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1141,16 +1145,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1160,16 +1164,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1179,16 +1183,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1198,16 +1202,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1217,16 +1221,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
     </row>
     <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1236,16 +1240,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -1255,16 +1259,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
     </row>
     <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1274,16 +1278,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
     </row>
     <row r="31" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -1293,16 +1297,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
     </row>
     <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1312,16 +1316,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -1331,16 +1335,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
     </row>
     <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1350,16 +1354,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
     </row>
     <row r="35" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -1369,16 +1373,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
     </row>
     <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1388,16 +1392,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
     </row>
     <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1407,16 +1411,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
     </row>
     <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1426,16 +1430,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
     </row>
     <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -1445,16 +1449,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
     </row>
     <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1464,16 +1468,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
     </row>
     <row r="41" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1483,16 +1487,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
     </row>
     <row r="42" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1502,16 +1506,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
     </row>
     <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -1521,16 +1525,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
     </row>
     <row r="44" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1540,16 +1544,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
     </row>
     <row r="45" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -1559,16 +1563,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
     </row>
     <row r="46" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -1578,16 +1582,16 @@
         <f>D46+E46+F46+G46+H46+I46+J46+L46</f>
         <v>0</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -1597,16 +1601,16 @@
         <f>D47+E47+F47+G47+H47+I47+J47+L47</f>
         <v>0</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
     </row>
     <row r="48" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
@@ -1618,14 +1622,14 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
     </row>
     <row r="49" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="G49" s="7"/>

</xml_diff>

<commit_message>
file name download changed
</commit_message>
<xml_diff>
--- a/Stat reports/Reports/Templates/Численность 6-Т для ПЭО.xlsx
+++ b/Stat reports/Reports/Templates/Численность 6-Т для ПЭО.xlsx
@@ -3,14 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Stat reports\Stat reports\Reports\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDFE850-68E8-459D-9B33-9A8CDDD3AC20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView yWindow="75" windowWidth="19440" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="19440" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="октябрь" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA[октябрь!$A$1:$L$50]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">октябрь!$A$1:$L$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -19,165 +25,164 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
-    <t xml:space="preserve">от 700 до 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ВСЕГО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Наименование
+    <t>от 700 до 900 руб.</t>
+  </si>
+  <si>
+    <t>ВСЕГО</t>
+  </si>
+  <si>
+    <t>Наименование
 показателя</t>
   </si>
   <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">свыше 8500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Начальник ПЭБ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">С.В. Володько</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 900,1 до 1 000 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 000,1 до 1 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 100,1 до 1 200 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 200,1 до 1 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 300,1 до 1 400 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 400,1 до 1 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 500,1 до 1 600 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 600,1 до 1 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 700,1 до 1 800 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 800,1 до 1 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 1 900,1 до 2 000 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 2 000,1 до 2 250 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 2 250,1 до 2 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 2 500,1 до 2 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 2 700,1 до 2 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 2 900,1 до 3 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 3 100,1 до 3 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 3 300,1 до 3 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 3 500,1 до 3 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 3 700,1 до 3 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 3 900,1 до 4 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 4 100,1 до 4 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 4 300,1 до 4 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 4 500,1 до 4 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 4 700,1 до 4 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 4 900,1 до 5 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 100,1 до 5 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 300,1 до 5 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 500,1 до 5 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 700,1 до 5 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 900,1 до 6 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 6 100,1 до 6 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 6 300,1 до 6 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 6 500,1 до 6 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 6 700,1 до 6 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 6 900,1 до 7 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 7 100,1 до 7 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 7 300,1 до 7 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 7 500,1 до 7 700 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 7 700,1 до 7 900 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 7 900,1 до 8 100 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 8 100,1 до 8 300 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 8 300,1 до 8 500 руб.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Информация о начисленной заработной плате рабочих филиалов со сдельной и сдельно-премиальной оплатой труда за</t>
+    <t>%</t>
+  </si>
+  <si>
+    <t>свыше 8500 руб.</t>
+  </si>
+  <si>
+    <t>Начальник ПЭБ</t>
+  </si>
+  <si>
+    <t>С.В. Володько</t>
+  </si>
+  <si>
+    <t>от 900,1 до 1 000 руб.</t>
+  </si>
+  <si>
+    <t>от 1 000,1 до 1 100 руб.</t>
+  </si>
+  <si>
+    <t>от 1 100,1 до 1 200 руб.</t>
+  </si>
+  <si>
+    <t>от 1 200,1 до 1 300 руб.</t>
+  </si>
+  <si>
+    <t>от 1 300,1 до 1 400 руб.</t>
+  </si>
+  <si>
+    <t>от 1 400,1 до 1 500 руб.</t>
+  </si>
+  <si>
+    <t>от 1 500,1 до 1 600 руб.</t>
+  </si>
+  <si>
+    <t>от 1 600,1 до 1 700 руб.</t>
+  </si>
+  <si>
+    <t>от 1 700,1 до 1 800 руб.</t>
+  </si>
+  <si>
+    <t>от 1 800,1 до 1 900 руб.</t>
+  </si>
+  <si>
+    <t>от 1 900,1 до 2 000 руб.</t>
+  </si>
+  <si>
+    <t>от 2 000,1 до 2 250 руб.</t>
+  </si>
+  <si>
+    <t>от 2 250,1 до 2 500 руб.</t>
+  </si>
+  <si>
+    <t>от 2 500,1 до 2 700 руб.</t>
+  </si>
+  <si>
+    <t>от 2 700,1 до 2 900 руб.</t>
+  </si>
+  <si>
+    <t>от 2 900,1 до 3 100 руб.</t>
+  </si>
+  <si>
+    <t>от 3 100,1 до 3 300 руб.</t>
+  </si>
+  <si>
+    <t>от 3 300,1 до 3 500 руб.</t>
+  </si>
+  <si>
+    <t>от 3 500,1 до 3 700 руб.</t>
+  </si>
+  <si>
+    <t>от 3 700,1 до 3 900 руб.</t>
+  </si>
+  <si>
+    <t>от 3 900,1 до 4 100 руб.</t>
+  </si>
+  <si>
+    <t>от 4 100,1 до 4 300 руб.</t>
+  </si>
+  <si>
+    <t>от 4 300,1 до 4 500 руб.</t>
+  </si>
+  <si>
+    <t>от 4 500,1 до 4 700 руб.</t>
+  </si>
+  <si>
+    <t>от 4 700,1 до 4 900 руб.</t>
+  </si>
+  <si>
+    <t>от 4 900,1 до 5 100 руб.</t>
+  </si>
+  <si>
+    <t>от 5 100,1 до 5 300 руб.</t>
+  </si>
+  <si>
+    <t>от 5 300,1 до 5 500 руб.</t>
+  </si>
+  <si>
+    <t>от 5 500,1 до 5 700 руб.</t>
+  </si>
+  <si>
+    <t>от 5 700,1 до 5 900 руб.</t>
+  </si>
+  <si>
+    <t>от 5 900,1 до 6 100 руб.</t>
+  </si>
+  <si>
+    <t>от 6 100,1 до 6 300 руб.</t>
+  </si>
+  <si>
+    <t>от 6 300,1 до 6 500 руб.</t>
+  </si>
+  <si>
+    <t>от 6 500,1 до 6 700 руб.</t>
+  </si>
+  <si>
+    <t>от 6 700,1 до 6 900 руб.</t>
+  </si>
+  <si>
+    <t>от 6 900,1 до 7 100 руб.</t>
+  </si>
+  <si>
+    <t>от 7 100,1 до 7 300 руб.</t>
+  </si>
+  <si>
+    <t>от 7 300,1 до 7 500 руб.</t>
+  </si>
+  <si>
+    <t>от 7 500,1 до 7 700 руб.</t>
+  </si>
+  <si>
+    <t>от 7 700,1 до 7 900 руб.</t>
+  </si>
+  <si>
+    <t>от 7 900,1 до 8 100 руб.</t>
+  </si>
+  <si>
+    <t>от 8 100,1 до 8 300 руб.</t>
+  </si>
+  <si>
+    <t>от 8 300,1 до 8 500 руб.</t>
+  </si>
+  <si>
+    <t>Информация о начисленной заработной плате рабочих филиалов со сдельной и сдельно-премиальной оплатой труда за</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -365,27 +370,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,6 +380,18 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -404,11 +400,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -671,7 +667,7 @@
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
-          <a:sp3d prstMaterial="warmMatte">
+          <a:sp3d>
             <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
@@ -734,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:M50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,20 +753,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -783,14 +779,14 @@
         <v>3</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -800,19 +796,19 @@
         <f t="shared" ref="B3:B45" si="0">D3+E3+F3+G3+H3+I3+J3+L3+K3</f>
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="e">
+      <c r="C3" s="16" t="e">
         <f>SUM(B3:B14)/B48</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -822,16 +818,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -841,16 +837,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -860,16 +856,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -879,16 +875,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -898,16 +894,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -917,16 +913,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -936,16 +932,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -955,16 +951,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -974,16 +970,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -993,16 +989,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1012,16 +1008,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1031,19 +1027,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C15" s="11" t="e">
+      <c r="C15" s="16" t="e">
         <f>SUM(B15:B21)/B48</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1053,16 +1049,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1072,16 +1068,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1091,16 +1087,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1110,16 +1106,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1129,16 +1125,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1148,16 +1144,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1167,19 +1163,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C22" s="11" t="e">
+      <c r="C22" s="16" t="e">
         <f>SUM(B22:B47)/B48</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1189,16 +1185,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1208,16 +1204,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1227,16 +1223,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1246,16 +1242,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1265,16 +1261,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1284,16 +1280,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -1303,16 +1299,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1322,16 +1318,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -1341,16 +1337,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1360,16 +1356,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -1379,16 +1375,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1398,16 +1394,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -1417,16 +1413,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1436,16 +1432,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1455,16 +1451,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1474,16 +1470,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -1493,16 +1489,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="17"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1512,16 +1508,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1531,16 +1527,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1550,16 +1546,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -1569,16 +1565,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="17"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1588,16 +1584,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -1607,16 +1603,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="17"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -1626,16 +1622,16 @@
         <f>D46+E46+F46+G46+H46+I46+J46+L46</f>
         <v>0</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -1645,16 +1641,16 @@
         <f>D47+E47+F47+G47+H47+I47+J47+L47</f>
         <v>0</v>
       </c>
-      <c r="C47" s="13"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
@@ -1666,14 +1662,14 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
     </row>
     <row r="49" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="G49" s="9"/>
@@ -1681,10 +1677,10 @@
       <c r="I49" s="9"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>5</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="H50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1695,7 +1691,7 @@
     <mergeCell ref="C3:C14"/>
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <pageMargins left="0.8661417322834646" right="0.31496062992125984" top="0.4724409448818898" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.86614173228346458" right="0.31496062992125984" top="0.47244094488188981" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>